<commit_message>
Large Max Growth fix
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_LargeMaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_LargeMaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E3AA05-BE5F-4FFB-883A-C69F3F3EE950}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42F5E08-F279-419B-BDED-80639CB23BF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -5706,7 +5706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89417C8F-9D07-4311-9372-0B0C534E50C4}">
   <dimension ref="A2:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
@@ -6581,7 +6581,7 @@
   <dimension ref="A2:N40"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7114,8 +7114,8 @@
         <v>185</v>
       </c>
       <c r="J16" s="29">
-        <f>1+C32</f>
-        <v>1.5</v>
+        <f>1-C32</f>
+        <v>0.5</v>
       </c>
       <c r="K16" s="2">
         <v>1</v>
@@ -7568,8 +7568,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A2:N26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9840,15 +9840,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -10059,6 +10050,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -10066,14 +10066,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10092,6 +10084,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
No Ker degrowth rate
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_LargeMaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_LargeMaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42F5E08-F279-419B-BDED-80639CB23BF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4197201D-3072-40A9-9E45-C422E1846D23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -174,7 +174,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="229">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -6578,10 +6578,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9933FEB4-63EA-406B-A848-C3344FC12632}">
-  <dimension ref="A2:N40"/>
+  <dimension ref="A2:N37"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6694,7 +6694,7 @@
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A24,"MaxGrowth",B24)</f>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A21,"MaxGrowth",B21)</f>
         <v>UC_RSD_MaxGrowth_AmbientHeat</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -6714,27 +6714,27 @@
         <v>15</v>
       </c>
       <c r="J6" s="29">
-        <f>1+C24</f>
+        <f>1+C21</f>
         <v>1.5</v>
       </c>
       <c r="K6" s="2">
         <v>1</v>
       </c>
       <c r="L6" s="16">
-        <f>-D24</f>
+        <f>-D21</f>
         <v>-0.3</v>
       </c>
       <c r="M6" s="2">
         <v>5</v>
       </c>
       <c r="N6" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A25, "maximum growth rate of",B25)</f>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A22, "maximum growth rate of",B22)</f>
         <v>RSD maximum growth rate of Biodiesel</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A25,"MaxGrowth",B25)</f>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A22,"MaxGrowth",B22)</f>
         <v>UC_RSD_MaxGrowth_Biodiesel</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -6754,27 +6754,27 @@
         <v>15</v>
       </c>
       <c r="J7" s="29">
-        <f>1+C25</f>
+        <f>1+C22</f>
         <v>1.5</v>
       </c>
       <c r="K7" s="2">
         <v>1</v>
       </c>
       <c r="L7" s="16">
-        <f>-D26</f>
+        <f>-D23</f>
         <v>0</v>
       </c>
       <c r="M7" s="2">
         <v>5</v>
       </c>
       <c r="N7" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A26, "maximum growth rate of",B26)</f>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A23, "maximum growth rate of",B23)</f>
         <v>RSD maximum growth rate of Biomass</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A26,"MaxGrowth",B26)</f>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A23,"MaxGrowth",B23)</f>
         <v>UC_RSD_MaxGrowth_Biomass</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -6794,27 +6794,27 @@
         <v>15</v>
       </c>
       <c r="J8" s="29">
-        <f>1+C26</f>
+        <f>1+C23</f>
         <v>1.5</v>
       </c>
       <c r="K8" s="2">
         <v>1</v>
       </c>
       <c r="L8" s="16">
-        <f>-D26</f>
+        <f>-D23</f>
         <v>0</v>
       </c>
       <c r="M8" s="2">
         <v>5</v>
       </c>
       <c r="N8" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A26, "maximum growth rate of",B26)</f>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A23, "maximum growth rate of",B23)</f>
         <v>RSD maximum growth rate of Biomass</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A27,"MaxGrowth",B27)</f>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A24,"MaxGrowth",B24)</f>
         <v>UC_RSD_MaxGrowth_Coal</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -6834,195 +6834,195 @@
         <v>15</v>
       </c>
       <c r="J9" s="29">
+        <f>1+C24</f>
+        <v>1.5</v>
+      </c>
+      <c r="K9" s="2">
+        <v>1</v>
+      </c>
+      <c r="L9" s="16">
+        <f>-D24</f>
+        <v>-0.3</v>
+      </c>
+      <c r="M9" s="2">
+        <v>5</v>
+      </c>
+      <c r="N9" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A24, "maximum growth rate of",B24)</f>
+        <v>RSD maximum growth rate of Coal</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A25,"MaxGrowth",B25)</f>
+        <v>UC_RSD_MaxGrowth_Peat</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="F10" t="s">
+        <v>206</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H10" s="2">
+        <v>2021</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="29">
+        <f>1+C25</f>
+        <v>1.5</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1</v>
+      </c>
+      <c r="L10" s="16">
+        <f>-D25</f>
+        <v>-0.3</v>
+      </c>
+      <c r="M10" s="2">
+        <v>5</v>
+      </c>
+      <c r="N10" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A25, "maximum growth rate of",B25)</f>
+        <v>RSD maximum growth rate of Peat</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A26,"MaxGrowth",B26)</f>
+        <v>UC_RSD_MaxGrowth_Electricity</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="F11" t="s">
+        <v>207</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H11" s="2">
+        <v>2021</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="29">
+        <f>1+C26</f>
+        <v>1.5</v>
+      </c>
+      <c r="K11" s="2">
+        <v>1</v>
+      </c>
+      <c r="L11" s="16">
+        <f>-D26</f>
+        <v>-0.1</v>
+      </c>
+      <c r="M11" s="2">
+        <v>5</v>
+      </c>
+      <c r="N11" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A26, "maximum growth rate of",B26)</f>
+        <v>RSD maximum growth rate of Electricity</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A27,"MaxGrowth",B27)</f>
+        <v>UC_RSD_MaxGrowth_Ethanol</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="F12" t="s">
+        <v>208</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H12" s="2">
+        <v>2021</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="29">
         <f>1+C27</f>
         <v>1.5</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K12" s="2">
         <v>1</v>
       </c>
-      <c r="L9" s="16">
+      <c r="L12" s="16">
         <f>-D27</f>
-        <v>-0.3</v>
-      </c>
-      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+      <c r="M12" s="2">
         <v>5</v>
       </c>
-      <c r="N9" s="2" t="str">
+      <c r="N12" s="2" t="str">
         <f>_xlfn.TEXTJOIN(" ",TRUE,A27, "maximum growth rate of",B27)</f>
-        <v>RSD maximum growth rate of Coal</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A27,"MaxDeGrowth",B27)</f>
-        <v>UC_RSD_MaxDeGrowth_Coal</v>
-      </c>
-      <c r="C10" s="2" t="s">
+        <v>RSD maximum growth rate of Ethanol</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A28,"MaxGrowth",B28)</f>
+        <v>UC_RSD_MaxGrowth_Gas</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="F10" t="s">
-        <v>205</v>
-      </c>
-      <c r="G10" s="2" t="s">
+      <c r="D13" s="2"/>
+      <c r="F13" t="s">
+        <v>209</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H13" s="2">
         <v>2021</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="J10" s="29">
-        <f>1-C27</f>
-        <v>0.5</v>
-      </c>
-      <c r="K10" s="2">
-        <v>1</v>
-      </c>
-      <c r="L10" s="16">
-        <f>-D28</f>
-        <v>-0.3</v>
-      </c>
-      <c r="M10" s="2">
-        <v>5</v>
-      </c>
-      <c r="N10" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A28, "maximum degrowth rate of",B27)</f>
-        <v>RSD maximum degrowth rate of Coal</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A28,"MaxGrowth",B28)</f>
-        <v>UC_RSD_MaxGrowth_Peat</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="F11" t="s">
-        <v>206</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="H11" s="2">
-        <v>2021</v>
-      </c>
-      <c r="I11" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J11" s="29">
+      <c r="J13" s="29">
         <f>1+C28</f>
         <v>1.5</v>
       </c>
-      <c r="K11" s="2">
-        <v>1</v>
-      </c>
-      <c r="L11" s="16">
-        <f>-D28</f>
-        <v>-0.3</v>
-      </c>
-      <c r="M11" s="2">
-        <v>5</v>
-      </c>
-      <c r="N11" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A28, "maximum growth rate of",B28)</f>
-        <v>RSD maximum growth rate of Peat</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A29,"MaxDeGrowth",B28)</f>
-        <v>UC_RSD_MaxDeGrowth_Peat</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="F12" t="s">
-        <v>206</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="H12" s="2">
-        <v>2021</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="J12" s="29">
-        <f>1-C28</f>
-        <v>0.5</v>
-      </c>
-      <c r="K12" s="2">
-        <v>1</v>
-      </c>
-      <c r="L12" s="16">
-        <f>-D29</f>
-        <v>-0.1</v>
-      </c>
-      <c r="M12" s="2">
-        <v>5</v>
-      </c>
-      <c r="N12" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A29, "maximum degrowth rate of",B28)</f>
-        <v>RSD maximum degrowth rate of Peat</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A29,"MaxGrowth",B29)</f>
-        <v>UC_RSD_MaxGrowth_Electricity</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="F13" t="s">
-        <v>207</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="H13" s="2">
-        <v>2021</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J13" s="29">
-        <f>1+C29</f>
-        <v>1.5</v>
-      </c>
       <c r="K13" s="2">
         <v>1</v>
       </c>
       <c r="L13" s="16">
-        <f>-D29</f>
+        <f>-D28</f>
         <v>-0.1</v>
       </c>
       <c r="M13" s="2">
         <v>5</v>
       </c>
       <c r="N13" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A29, "maximum growth rate of",B29)</f>
-        <v>RSD maximum growth rate of Electricity</v>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A28, "maximum growth rate of",B28)</f>
+        <v>RSD maximum growth rate of Gas</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A30,"MaxGrowth",B30)</f>
-        <v>UC_RSD_MaxGrowth_Ethanol</v>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A29,"MinGrowth",B29)</f>
+        <v>UC_RSD_MinGrowth_DistrictHeat</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>144</v>
       </c>
       <c r="D14" s="2"/>
       <c r="F14" t="s">
-        <v>208</v>
+        <v>221</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>142</v>
@@ -7031,38 +7031,38 @@
         <v>2021</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>15</v>
+        <v>185</v>
       </c>
       <c r="J14" s="29">
-        <f>1+C30</f>
-        <v>1.5</v>
+        <f>1-C29</f>
+        <v>0.5</v>
       </c>
       <c r="K14" s="2">
         <v>1</v>
       </c>
       <c r="L14" s="16">
         <f>-D30</f>
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="M14" s="2">
         <v>5</v>
       </c>
       <c r="N14" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A30, "maximum growth rate of",B30)</f>
-        <v>RSD maximum growth rate of Ethanol</v>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A29, "minimum growth rate of",B29)</f>
+        <v>RSD minimum growth rate of DistrictHeat</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A31,"MaxGrowth",B31)</f>
-        <v>UC_RSD_MaxGrowth_Gas</v>
+        <f t="shared" ref="B15:B16" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A30,"MaxGrowth",B30)</f>
+        <v>UC_RSD_MaxGrowth_LPG</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>144</v>
       </c>
       <c r="D15" s="2"/>
       <c r="F15" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>142</v>
@@ -7074,35 +7074,35 @@
         <v>15</v>
       </c>
       <c r="J15" s="29">
-        <f>1+C31</f>
+        <f t="shared" ref="J15:J16" si="1">1+C30</f>
         <v>1.5</v>
       </c>
       <c r="K15" s="2">
         <v>1</v>
       </c>
       <c r="L15" s="16">
-        <f>-D31</f>
+        <f t="shared" ref="L15:L16" si="2">-D30</f>
         <v>-0.1</v>
       </c>
       <c r="M15" s="2">
         <v>5</v>
       </c>
       <c r="N15" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A31, "maximum growth rate of",B31)</f>
-        <v>RSD maximum growth rate of Gas</v>
+        <f t="shared" ref="N15:N16" si="3">_xlfn.TEXTJOIN(" ",TRUE,A30, "maximum growth rate of",B30)</f>
+        <v>RSD maximum growth rate of LPG</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A32,"MinGrowth",B32)</f>
-        <v>UC_RSD_MinGrowth_DistrictHeat</v>
+        <f t="shared" si="0"/>
+        <v>UC_RSD_MaxGrowth_Kerosene</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>144</v>
       </c>
       <c r="D16" s="2"/>
       <c r="F16" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>142</v>
@@ -7111,38 +7111,38 @@
         <v>2021</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>185</v>
+        <v>15</v>
       </c>
       <c r="J16" s="29">
-        <f>1-C32</f>
-        <v>0.5</v>
+        <f t="shared" si="1"/>
+        <v>1.5</v>
       </c>
       <c r="K16" s="2">
         <v>1</v>
       </c>
       <c r="L16" s="16">
-        <f>-D33</f>
+        <f t="shared" si="2"/>
         <v>-0.1</v>
       </c>
       <c r="M16" s="2">
         <v>5</v>
       </c>
       <c r="N16" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A32, "minimum growth rate of",B32)</f>
-        <v>RSD minimum growth rate of DistrictHeat</v>
+        <f t="shared" si="3"/>
+        <v>RSD maximum growth rate of Kerosene</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="str">
-        <f t="shared" ref="B17:B18" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A33,"MaxGrowth",B33)</f>
-        <v>UC_RSD_MaxGrowth_LPG</v>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A32,"MaxGrowth",B32)</f>
+        <v>UC_RSD_MaxGrowth_Solar</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>144</v>
       </c>
       <c r="D17" s="2"/>
       <c r="F17" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>142</v>
@@ -7154,35 +7154,35 @@
         <v>15</v>
       </c>
       <c r="J17" s="29">
-        <f t="shared" ref="J17:J18" si="1">1+C33</f>
+        <f>1+C32</f>
         <v>1.5</v>
       </c>
       <c r="K17" s="2">
         <v>1</v>
       </c>
       <c r="L17" s="16">
-        <f t="shared" ref="L17:L18" si="2">-D33</f>
-        <v>-0.1</v>
+        <f>-D32</f>
+        <v>-0.2</v>
       </c>
       <c r="M17" s="2">
         <v>5</v>
       </c>
       <c r="N17" s="2" t="str">
-        <f t="shared" ref="N17:N18" si="3">_xlfn.TEXTJOIN(" ",TRUE,A33, "maximum growth rate of",B33)</f>
-        <v>RSD maximum growth rate of LPG</v>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A32, "maximum growth rate of",B32)</f>
+        <v>RSD maximum growth rate of Solar</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UC_RSD_MaxGrowth_Kerosene</v>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A32,"MinGrowth",B32)</f>
+        <v>UC_RSD_MinGrowth_Solar</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>144</v>
       </c>
       <c r="D18" s="2"/>
       <c r="F18" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>142</v>
@@ -7191,153 +7191,75 @@
         <v>2021</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>15</v>
+        <v>185</v>
       </c>
       <c r="J18" s="29">
-        <f t="shared" si="1"/>
-        <v>1.5</v>
+        <f>1+C32/25</f>
+        <v>1.02</v>
       </c>
       <c r="K18" s="2">
         <v>1</v>
       </c>
       <c r="L18" s="16">
-        <f t="shared" si="2"/>
-        <v>-0.1</v>
+        <f>-D32</f>
+        <v>-0.2</v>
       </c>
       <c r="M18" s="2">
         <v>5</v>
       </c>
       <c r="N18" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>RSD maximum growth rate of Kerosene</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A34,"MaxDegrowth",B34)</f>
-        <v>UC_RSD_MaxDegrowth_Kerosene</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="F19" t="s">
-        <v>211</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="H19" s="2">
-        <v>2021</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="J19" s="29">
-        <f>1-C34</f>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A32, "minimum growth rate of",B32)</f>
+        <v>RSD minimum growth rate of Solar</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>117</v>
+      </c>
+      <c r="D20" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>194</v>
+      </c>
+      <c r="B21" t="s">
+        <v>190</v>
+      </c>
+      <c r="C21" s="50">
         <v>0.5</v>
       </c>
-      <c r="K19" s="2">
-        <v>1</v>
-      </c>
-      <c r="L19" s="16">
-        <f>-D34</f>
-        <v>-0.1</v>
-      </c>
-      <c r="M19" s="2">
-        <v>5</v>
-      </c>
-      <c r="N19" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A34, "maximum degrowth rate of",B34)</f>
-        <v>RSD maximum degrowth rate of Kerosene</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A35,"MaxGrowth",B35)</f>
-        <v>UC_RSD_MaxGrowth_Solar</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D20" s="2"/>
-      <c r="F20" t="s">
-        <v>212</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="H20" s="2">
-        <v>2021</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J20" s="29">
-        <f>1+C35</f>
-        <v>1.5</v>
-      </c>
-      <c r="K20" s="2">
-        <v>1</v>
-      </c>
-      <c r="L20" s="16">
-        <f>-D35</f>
-        <v>-0.2</v>
-      </c>
-      <c r="M20" s="2">
-        <v>5</v>
-      </c>
-      <c r="N20" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A35, "maximum growth rate of",B35)</f>
-        <v>RSD maximum growth rate of Solar</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A35,"MinGrowth",B35)</f>
-        <v>UC_RSD_MinGrowth_Solar</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D21" s="2"/>
-      <c r="F21" t="s">
-        <v>212</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="H21" s="2">
-        <v>2021</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="J21" s="29">
-        <f>1+C35/25</f>
-        <v>1.02</v>
-      </c>
-      <c r="K21" s="2">
-        <v>1</v>
-      </c>
-      <c r="L21" s="16">
-        <f>-D35</f>
-        <v>-0.2</v>
-      </c>
-      <c r="M21" s="2">
-        <v>5</v>
-      </c>
-      <c r="N21" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A35, "minimum growth rate of",B35)</f>
-        <v>RSD minimum growth rate of Solar</v>
+      <c r="D21">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>194</v>
+      </c>
+      <c r="B22" t="s">
+        <v>196</v>
+      </c>
+      <c r="C22" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>117</v>
-      </c>
-      <c r="D23" t="s">
-        <v>189</v>
+      <c r="A23" t="s">
+        <v>194</v>
+      </c>
+      <c r="B23" t="s">
+        <v>137</v>
+      </c>
+      <c r="C23" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -7345,7 +7267,7 @@
         <v>194</v>
       </c>
       <c r="B24" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="C24" s="50">
         <v>0.5</v>
@@ -7359,13 +7281,13 @@
         <v>194</v>
       </c>
       <c r="B25" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C25" s="50">
         <v>0.5</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -7373,13 +7295,13 @@
         <v>194</v>
       </c>
       <c r="B26" t="s">
-        <v>137</v>
+        <v>199</v>
       </c>
       <c r="C26" s="50">
         <v>0.5</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -7387,13 +7309,13 @@
         <v>194</v>
       </c>
       <c r="B27" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C27" s="50">
         <v>0.5</v>
       </c>
       <c r="D27">
-        <v>0.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -7401,13 +7323,13 @@
         <v>194</v>
       </c>
       <c r="B28" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C28" s="50">
         <v>0.5</v>
       </c>
       <c r="D28">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -7415,13 +7337,13 @@
         <v>194</v>
       </c>
       <c r="B29" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="C29" s="50">
         <v>0.5</v>
       </c>
       <c r="D29">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -7429,13 +7351,13 @@
         <v>194</v>
       </c>
       <c r="B30" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C30" s="50">
         <v>0.5</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -7443,7 +7365,7 @@
         <v>194</v>
       </c>
       <c r="B31" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="C31" s="50">
         <v>0.5</v>
@@ -7457,105 +7379,63 @@
         <v>194</v>
       </c>
       <c r="B32" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="C32" s="50">
         <v>0.5</v>
       </c>
       <c r="D32">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>194</v>
-      </c>
-      <c r="B33" t="s">
-        <v>201</v>
-      </c>
-      <c r="C33" s="50">
-        <v>0.5</v>
-      </c>
-      <c r="D33">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>194</v>
-      </c>
-      <c r="B34" t="s">
-        <v>202</v>
-      </c>
-      <c r="C34" s="50">
-        <v>0.5</v>
-      </c>
-      <c r="D34">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>194</v>
-      </c>
-      <c r="B35" t="s">
-        <v>203</v>
-      </c>
-      <c r="C35" s="50">
-        <v>0.5</v>
-      </c>
-      <c r="D35">
         <v>0.2</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="45" t="s">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="45" t="s">
         <v>213</v>
       </c>
-      <c r="H38" s="46"/>
-    </row>
-    <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="47" t="s">
+      <c r="H35" s="46"/>
+    </row>
+    <row r="36" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="47" t="s">
         <v>214</v>
       </c>
-      <c r="C39" s="47" t="s">
+      <c r="C36" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="D39" s="47" t="s">
+      <c r="D36" s="47" t="s">
         <v>215</v>
       </c>
-      <c r="E39" s="47" t="s">
+      <c r="E36" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F39" s="48" t="str">
+      <c r="F36" s="48" t="str">
         <f>IF([1]Regions!C$3&lt;&gt;"",[1]Regions!C$3,"*")</f>
         <v>IE</v>
       </c>
-      <c r="G39" s="48" t="str">
+      <c r="G36" s="48" t="str">
         <f>IF([1]Regions!C$3&lt;&gt;"",[1]Regions!D$3,"*")</f>
         <v>National</v>
       </c>
-      <c r="H39" s="49" t="s">
+      <c r="H36" s="49" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D40" t="s">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
         <v>217</v>
       </c>
-      <c r="E40">
+      <c r="E37">
         <v>2018</v>
       </c>
-      <c r="F40">
+      <c r="F37">
         <v>2222</v>
       </c>
-      <c r="G40">
-        <f>F40</f>
+      <c r="G37">
+        <f>F37</f>
         <v>2222</v>
       </c>
-      <c r="H40" t="str">
-        <f xml:space="preserve"> _xlfn.TEXTJOIN(",",TRUE,F6:F21)</f>
-        <v>RSDAHT,RSDAHT2,RSDBDL,RSDWOO,RSDCOA,RSDCOA,RSDPEA,RSDPEA,RSDELC,RSDETH,RSDGAS,RSDHET*,RSDLPG,RSDKER,RSDKER,RSDSOL,RSDSOL</v>
+      <c r="H37" t="str">
+        <f xml:space="preserve"> _xlfn.TEXTJOIN(",",TRUE,F6:F18)</f>
+        <v>RSDAHT,RSDAHT2,RSDBDL,RSDWOO,RSDCOA,RSDPEA,RSDELC,RSDETH,RSDGAS,RSDHET*,RSDLPG,RSDKER,RSDSOL,RSDSOL</v>
       </c>
     </row>
   </sheetData>
@@ -7568,7 +7448,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A2:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
@@ -9840,6 +9720,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -10050,22 +9945,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10082,21 +9979,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>